<commit_message>
with the most up-to-date mapping defs from s3
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farzanfatemifar/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61B0C24-B42D-6543-8D78-46711B88E9E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="27420" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="notify_type_lookup" sheetId="11" r:id="rId1"/>
@@ -25,8 +24,11 @@
     <sheet name="deputy_death_notifications" sheetId="8" r:id="rId10"/>
     <sheet name="deputy_date_of_death_lookup" sheetId="9" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,9 +38,6 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="71">
   <si>
     <t>casrec_code</t>
   </si>
@@ -209,9 +208,6 @@
   </si>
   <si>
     <t>Disch Death</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
   <si>
     <t>Y</t>
@@ -268,11 +264,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -754,19 +750,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,7 +796,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>4</v>
       </c>
@@ -809,7 +805,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -832,7 +828,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>6</v>
       </c>
@@ -841,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -864,7 +860,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -873,7 +869,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -896,7 +892,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -905,7 +901,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
@@ -928,7 +924,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -937,7 +933,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
@@ -960,7 +956,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
@@ -968,7 +964,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
@@ -991,7 +987,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="15">
+    <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -999,7 +995,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1022,7 +1018,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1048,7 +1044,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1056,7 +1052,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1065,7 +1061,7 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5:O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -1087,7 +1083,7 @@
     <col min="18" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1140,7 +1136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1161,7 +1157,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1185,7 +1181,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1216,7 +1212,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15">
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1248,7 +1244,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1280,7 +1276,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15">
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -1312,7 +1308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15">
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1342,7 +1338,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1372,7 +1368,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15">
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1402,7 +1398,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1432,7 +1428,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1440,19 +1436,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +1482,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>99</v>
       </c>
@@ -1518,7 +1514,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -1543,7 +1539,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1569,7 +1565,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1595,7 +1591,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1621,7 +1617,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1647,7 +1643,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1669,7 +1665,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1695,7 +1691,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1703,19 +1699,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1749,13 +1745,13 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="5" t="b">
         <v>1</v>
@@ -1781,13 +1777,13 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="6" t="b">
         <v>0</v>
@@ -1813,7 +1809,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1835,7 +1831,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1861,7 +1857,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1887,7 +1883,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1913,7 +1909,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1935,7 +1931,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1961,7 +1957,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1969,19 +1965,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2015,7 +2011,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2047,7 +2043,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2073,7 +2069,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2095,7 +2091,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2121,7 +2117,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2147,7 +2143,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2173,7 +2169,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2195,7 +2191,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2221,7 +2217,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -2229,19 +2225,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2275,7 +2271,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2307,7 +2303,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2333,7 +2329,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -2359,7 +2355,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2385,7 +2381,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2411,7 +2407,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2433,7 +2429,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2455,7 +2451,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2481,7 +2477,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -2489,19 +2485,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2535,13 +2531,13 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -2567,16 +2563,16 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -2599,16 +2595,16 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -2631,7 +2627,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2657,7 +2653,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2679,7 +2675,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2705,7 +2701,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2727,7 +2723,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2753,7 +2749,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -2761,19 +2757,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2807,16 +2803,16 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2839,16 +2835,16 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -2871,12 +2867,12 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>49</v>
@@ -2902,7 +2898,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2928,7 +2924,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2950,7 +2946,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2976,7 +2972,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2998,7 +2994,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3024,7 +3020,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3032,19 +3028,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3078,7 +3074,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3110,7 +3106,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -3136,7 +3132,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3162,7 +3158,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -3184,7 +3180,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3210,7 +3206,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3236,7 +3232,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3258,7 +3254,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3284,7 +3280,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3292,19 +3288,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3338,7 +3334,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3370,7 +3366,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -3392,7 +3388,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3418,7 +3414,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3444,7 +3440,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3470,7 +3466,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3496,7 +3492,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3518,7 +3514,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3544,7 +3540,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3552,15 +3548,15 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -3582,7 +3578,7 @@
     <col min="18" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -3635,7 +3631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -3656,7 +3652,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -3680,7 +3676,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -3712,7 +3708,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15">
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -3744,7 +3740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -3769,10 +3765,10 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -3804,7 +3800,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16">
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -3829,7 +3825,7 @@
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -3838,7 +3834,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -3866,7 +3862,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16">
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -3891,7 +3887,7 @@
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -3900,7 +3896,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -3917,9 +3913,7 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="H11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="12"/>
@@ -3932,7 +3926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
update mapping defs from s3
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farzanfatemifar/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61B0C24-B42D-6543-8D78-46711B88E9E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="27420" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="notify_type_lookup" sheetId="11" r:id="rId1"/>
@@ -25,8 +24,11 @@
     <sheet name="deputy_death_notifications" sheetId="8" r:id="rId10"/>
     <sheet name="deputy_date_of_death_lookup" sheetId="9" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,9 +38,6 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="71">
   <si>
     <t>casrec_code</t>
   </si>
@@ -209,9 +208,6 @@
   </si>
   <si>
     <t>Disch Death</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
   <si>
     <t>Y</t>
@@ -268,11 +264,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -754,19 +750,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,7 +796,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>4</v>
       </c>
@@ -809,7 +805,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -832,7 +828,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>6</v>
       </c>
@@ -841,7 +837,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -864,7 +860,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -873,7 +869,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -896,7 +892,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -905,7 +901,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
@@ -928,7 +924,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -937,7 +933,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
@@ -960,7 +956,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
@@ -968,7 +964,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
@@ -991,7 +987,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="15">
+    <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -999,7 +995,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1022,7 +1018,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1048,7 +1044,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1056,7 +1052,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1065,7 +1061,7 @@
       <selection pane="bottomLeft" activeCell="O5" sqref="O5:O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -1087,7 +1083,7 @@
     <col min="18" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1140,7 +1136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1161,7 +1157,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1185,7 +1181,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1216,7 +1212,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15">
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1248,7 +1244,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1280,7 +1276,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15">
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -1312,7 +1308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15">
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1342,7 +1338,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1372,7 +1368,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15">
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1402,7 +1398,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1432,7 +1428,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1440,19 +1436,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +1482,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>99</v>
       </c>
@@ -1518,7 +1514,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -1543,7 +1539,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1569,7 +1565,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1595,7 +1591,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1621,7 +1617,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1647,7 +1643,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1669,7 +1665,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1695,7 +1691,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1703,19 +1699,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1749,13 +1745,13 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="5" t="b">
         <v>1</v>
@@ -1781,13 +1777,13 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="6" t="b">
         <v>0</v>
@@ -1813,7 +1809,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1835,7 +1831,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1861,7 +1857,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1887,7 +1883,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1913,7 +1909,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1935,7 +1931,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1961,7 +1957,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -1969,19 +1965,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2015,7 +2011,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2047,7 +2043,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2073,7 +2069,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2095,7 +2091,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2121,7 +2117,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2147,7 +2143,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2173,7 +2169,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2195,7 +2191,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2221,7 +2217,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -2229,19 +2225,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2275,7 +2271,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2307,7 +2303,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2333,7 +2329,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -2359,7 +2355,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2385,7 +2381,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2411,7 +2407,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2433,7 +2429,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2455,7 +2451,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2481,7 +2477,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -2489,19 +2485,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2535,13 +2531,13 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -2567,16 +2563,16 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -2599,16 +2595,16 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -2631,7 +2627,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2657,7 +2653,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2679,7 +2675,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2705,7 +2701,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2727,7 +2723,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2753,7 +2749,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -2761,19 +2757,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2807,16 +2803,16 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2839,16 +2835,16 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -2871,12 +2867,12 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>49</v>
@@ -2902,7 +2898,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2928,7 +2924,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2950,7 +2946,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2976,7 +2972,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2998,7 +2994,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3024,7 +3020,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3032,19 +3028,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3078,7 +3074,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3110,7 +3106,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -3136,7 +3132,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3162,7 +3158,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -3184,7 +3180,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3210,7 +3206,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3236,7 +3232,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3258,7 +3254,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3284,7 +3280,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3292,19 +3288,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3338,7 +3334,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3370,7 +3366,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -3392,7 +3388,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3418,7 +3414,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3444,7 +3440,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3470,7 +3466,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3496,7 +3492,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3518,7 +3514,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3544,7 +3540,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3552,15 +3548,15 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -3582,7 +3578,7 @@
     <col min="18" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -3635,7 +3631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -3656,7 +3652,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -3680,7 +3676,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -3712,7 +3708,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15">
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -3744,7 +3740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -3769,10 +3765,10 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -3804,7 +3800,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16">
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -3829,7 +3825,7 @@
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -3838,7 +3834,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -3866,7 +3862,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16">
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -3891,7 +3887,7 @@
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -3900,7 +3896,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -3917,9 +3913,7 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="H11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="12"/>
@@ -3932,7 +3926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
IN-1002 fix proofofdeath (#434)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1506B7E9-CDA4-104E-AD18-67BAA36F2BC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="34400" windowHeight="21940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="460" windowWidth="34400" windowHeight="21940" tabRatio="500" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="13" r:id="rId1"/>
     <sheet name="notify_type_lookup" sheetId="11" r:id="rId2"/>
-    <sheet name="proof__boolean_lookup" sheetId="10" r:id="rId3"/>
+    <sheet name="proof_boolean_lookup" sheetId="10" r:id="rId3"/>
     <sheet name="proof_lookup" sheetId="4" r:id="rId4"/>
     <sheet name="notify_lookup" sheetId="1" r:id="rId5"/>
     <sheet name="termby_type_lookup" sheetId="12" r:id="rId6"/>
@@ -26,8 +20,11 @@
     <sheet name="deputy_death_notifications" sheetId="8" r:id="rId11"/>
     <sheet name="deputy_date_of_death_lookup" sheetId="9" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -37,9 +34,6 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -48,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="89">
   <si>
     <t>casrec_code</t>
   </si>
@@ -312,16 +306,19 @@
   </si>
   <si>
     <t>Stat,Deputy No</t>
+  </si>
+  <si>
+    <t>proof_boolean_lookup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -594,7 +591,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -629,7 +626,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -806,21 +803,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3265ACFE-72FF-7E41-81EA-89C110F66BD3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
@@ -848,7 +850,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28">
+    <row r="2" spans="1:8">
       <c r="A2" s="16" t="s">
         <v>85</v>
       </c>
@@ -871,7 +873,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28">
+    <row r="3" spans="1:8">
       <c r="A3" s="16" t="s">
         <v>83</v>
       </c>
@@ -896,19 +898,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -983,7 +990,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:17" ht="14">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1004,7 +1011,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:17" ht="14">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1028,7 +1035,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" ht="14">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1052,15 +1059,17 @@
         <v>9</v>
       </c>
       <c r="K4" s="5"/>
-      <c r="L4" s="15"/>
+      <c r="L4" s="15" t="s">
+        <v>88</v>
+      </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="14">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1092,7 +1101,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:17" ht="14">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1120,7 +1129,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15">
+    <row r="7" spans="1:17" ht="14">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -1152,7 +1161,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16">
+    <row r="8" spans="1:17" ht="14">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1186,7 +1195,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
+    <row r="9" spans="1:17" ht="14">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1214,7 +1223,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16">
+    <row r="10" spans="1:17" ht="14">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17" ht="14">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1282,20 +1291,25 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5:O10"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -1370,7 +1384,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:17" ht="14">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1391,7 +1405,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:17" ht="14">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1415,7 +1429,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" ht="14">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1446,7 +1460,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15">
+    <row r="5" spans="1:17" ht="14">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1572,7 +1586,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
+    <row r="9" spans="1:17" ht="14">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1632,7 +1646,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17" ht="14">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1666,18 +1680,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -1716,7 +1735,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="14">
       <c r="A2" s="2">
         <v>99</v>
       </c>
@@ -1748,7 +1767,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="14">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -1773,7 +1792,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="14">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1799,7 +1818,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="14">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1825,7 +1844,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="14">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1851,7 +1870,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="14">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1877,7 +1896,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="13">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1929,18 +1948,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -1979,7 +2003,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="14">
       <c r="A2" s="4">
         <v>4</v>
       </c>
@@ -2011,7 +2035,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="14">
       <c r="A3" s="4">
         <v>6</v>
       </c>
@@ -2043,7 +2067,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="14">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2075,7 +2099,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="14">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -2107,7 +2131,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="14">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2139,7 +2163,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="14">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2170,7 +2194,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="15">
+    <row r="8" spans="1:24" ht="14">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2231,20 +2255,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1025" width="14.5" customWidth="1"/>
+    <col min="1" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15" customHeight="1">
@@ -2281,7 +2312,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="14">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -2313,7 +2344,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="14">
       <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
@@ -2345,7 +2376,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="14">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2367,7 +2398,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="14">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2393,7 +2424,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="14">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2419,7 +2450,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="14">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2445,7 +2476,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="13">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2497,18 +2528,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -2547,7 +2583,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="14">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2579,7 +2615,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="14">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2605,7 +2641,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="14">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2627,7 +2663,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="14">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2653,7 +2689,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="14">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2679,7 +2715,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="14">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2705,7 +2741,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="13">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2757,18 +2793,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -2807,7 +2848,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="14">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2839,7 +2880,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="14">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2865,7 +2906,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="14">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -2891,7 +2932,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="14">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2917,7 +2958,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="14">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2943,7 +2984,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="14">
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2965,7 +3006,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="13">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3017,18 +3058,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -3067,7 +3113,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="14">
       <c r="A2" s="4" t="s">
         <v>60</v>
       </c>
@@ -3099,7 +3145,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="14">
       <c r="A3" s="4" t="s">
         <v>61</v>
       </c>
@@ -3131,7 +3177,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="14">
       <c r="A4" s="4" t="s">
         <v>62</v>
       </c>
@@ -3163,7 +3209,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="14">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3189,7 +3235,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="14">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -3211,7 +3257,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="14">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3237,7 +3283,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="13">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3289,18 +3335,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -3339,7 +3390,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="14">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3371,7 +3422,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="14">
       <c r="A3" s="4" t="s">
         <v>69</v>
       </c>
@@ -3403,7 +3454,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="14">
       <c r="A4" s="16" t="s">
         <v>70</v>
       </c>
@@ -3434,7 +3485,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="14">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3460,7 +3511,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="14">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -3482,7 +3533,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="14">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3508,7 +3559,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="13">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3560,18 +3611,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -3610,7 +3666,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="14">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3642,7 +3698,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="14">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -3668,7 +3724,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="14">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3694,7 +3750,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="14">
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -3716,7 +3772,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="14">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3742,7 +3798,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="14">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3768,7 +3824,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="13">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3820,18 +3876,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -3870,7 +3931,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24" ht="14">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3902,7 +3963,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24" ht="14">
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -3924,7 +3985,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24" ht="14">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3950,7 +4011,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24" ht="14">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3976,7 +4037,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15">
+    <row r="6" spans="1:24" ht="14">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -4002,7 +4063,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15">
+    <row r="7" spans="1:24" ht="14">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -4028,7 +4089,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="14">
+    <row r="8" spans="1:24" ht="13">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -4080,5 +4141,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
IN-1002b death notification fixes (#450)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="34400" windowHeight="21940" tabRatio="500" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="1440" yWindow="460" windowWidth="34400" windowHeight="21940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="13" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="92">
   <si>
     <t>casrec_code</t>
   </si>
@@ -309,6 +309,15 @@
   </si>
   <si>
     <t>proof_boolean_lookup</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -318,7 +327,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -367,6 +376,11 @@
       <color rgb="FF333333"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -429,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -463,6 +477,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,7 +818,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -910,7 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
@@ -1958,10 +1973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X1048576"/>
+  <dimension ref="A1:X1048569"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
@@ -2003,18 +2018,18 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15" customHeight="1">
       <c r="A2" s="4">
         <v>4</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="2"/>
+      <c r="D2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="8"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -2037,221 +2052,41 @@
     </row>
     <row r="3" spans="1:24" ht="14">
       <c r="A3" s="4">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
     </row>
     <row r="4" spans="1:24" ht="14">
       <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
+      <c r="D4" s="19" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="5" spans="1:24" ht="14">
-      <c r="A5" s="4">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+      <c r="A5" s="19">
+        <v>1</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-    </row>
-    <row r="6" spans="1:24" ht="14">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-    </row>
-    <row r="7" spans="1:24" ht="14">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-    </row>
-    <row r="8" spans="1:24" ht="14">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-    </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-    </row>
-    <row r="1048576" ht="15.75" customHeight="1"/>
+      <c r="D5" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="1048569" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Remove deputy death notification fields
As per IN-1092.
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C330B1-457E-CC44-B08F-956DE88487A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="34400" windowHeight="21940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-35600" yWindow="1360" windowWidth="34400" windowHeight="19900" tabRatio="500" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="13" r:id="rId1"/>
@@ -20,11 +26,8 @@
     <sheet name="deputy_death_notifications" sheetId="8" r:id="rId11"/>
     <sheet name="deputy_date_of_death_lookup" sheetId="9" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -34,6 +37,9 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -42,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="91">
   <si>
     <t>casrec_code</t>
   </si>
@@ -188,18 +194,12 @@
     <t>Migrated</t>
   </si>
   <si>
-    <t>Deputy</t>
-  </si>
-  <si>
     <t>OTHER</t>
   </si>
   <si>
     <t>Migration</t>
   </si>
   <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
     <t>DECEASED</t>
   </si>
   <si>
@@ -318,16 +318,19 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -443,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -478,6 +481,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,21 +828,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="20.5" customWidth="1"/>
@@ -841,74 +851,74 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="14">
+      <c r="A2" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>77</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>79</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="H2" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14">
+      <c r="A3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="16" t="s">
-        <v>83</v>
-      </c>
       <c r="B3" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -922,7 +932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -930,7 +940,7 @@
       <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -1005,7 +1015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14">
+    <row r="2" spans="1:17" ht="15">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1026,7 +1036,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14">
+    <row r="3" spans="1:17" ht="15">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1050,7 +1060,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14">
+    <row r="4" spans="1:17" ht="16">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1075,7 +1085,7 @@
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
@@ -1084,7 +1094,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="14">
+    <row r="5" spans="1:17" ht="15">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1116,7 +1126,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="14">
+    <row r="6" spans="1:17" ht="15">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1144,7 +1154,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="14">
+    <row r="7" spans="1:17" ht="15">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -1176,7 +1186,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="14">
+    <row r="8" spans="1:17" ht="16">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1201,7 +1211,7 @@
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -1210,7 +1220,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14">
+    <row r="9" spans="1:17" ht="15">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1238,7 +1248,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14">
+    <row r="10" spans="1:17" ht="16">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1263,7 +1273,7 @@
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -1272,7 +1282,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="14">
+    <row r="11" spans="1:17" ht="15">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1315,16 +1325,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -1338,7 +1348,7 @@
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="22.5" customWidth="1"/>
     <col min="12" max="12" width="20.5" customWidth="1"/>
-    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="13" max="13" width="17.5" style="21" customWidth="1"/>
     <col min="14" max="14" width="20.5" customWidth="1"/>
     <col min="15" max="15" width="18.33203125" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" customWidth="1"/>
@@ -1383,7 +1393,7 @@
       <c r="L1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="20" t="s">
         <v>22</v>
       </c>
       <c r="N1" s="9" t="s">
@@ -1399,7 +1409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14">
+    <row r="2" spans="1:17" ht="15">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1420,7 +1430,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14">
+    <row r="3" spans="1:17" ht="15">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1444,7 +1454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14">
+    <row r="4" spans="1:17" ht="15">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1465,17 +1475,16 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="12"/>
-      <c r="M4" s="5" t="b">
-        <f>TRUE()</f>
+      <c r="M4" s="22" t="b">
         <v>1</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1492,19 +1501,15 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="H5" s="5"/>
+      <c r="J5" s="6"/>
       <c r="K5" s="5"/>
       <c r="L5" s="13"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15">
@@ -1524,19 +1529,15 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="H6" s="5"/>
+      <c r="J6" s="6"/>
       <c r="K6" s="5"/>
       <c r="L6" s="14"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15">
@@ -1556,19 +1557,15 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="H7" s="5"/>
+      <c r="J7" s="6"/>
       <c r="K7" s="5"/>
       <c r="L7" s="14"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15">
@@ -1593,15 +1590,15 @@
       <c r="K8" s="5"/>
       <c r="L8" s="14"/>
       <c r="M8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1623,12 +1620,12 @@
       <c r="K9" s="5"/>
       <c r="L9" s="12"/>
       <c r="M9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="4" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15">
@@ -1652,16 +1649,14 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="14"/>
-      <c r="M10" s="5" t="s">
-        <v>51</v>
-      </c>
+      <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="14">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1688,7 +1683,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
     </row>
     <row r="1048576" ht="15.75" customHeight="1"/>
@@ -1704,14 +1699,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -1750,16 +1745,16 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="2">
         <v>99</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1782,7 +1777,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -1807,7 +1802,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1833,7 +1828,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1859,7 +1854,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1885,7 +1880,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1911,7 +1906,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1972,14 +1967,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X1048569"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -2027,7 +2022,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="2"/>
@@ -2050,7 +2045,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4">
         <v>3</v>
       </c>
@@ -2059,10 +2054,10 @@
         <v>5</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="14">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -2071,7 +2066,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="14">
@@ -2083,7 +2078,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="1048569" ht="15.75" customHeight="1"/>
@@ -2099,14 +2094,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
@@ -2147,13 +2142,13 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D2" s="5" t="b">
         <v>1</v>
@@ -2179,13 +2174,13 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="6" t="b">
         <v>0</v>
@@ -2211,7 +2206,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2233,7 +2228,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2259,7 +2254,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2285,7 +2280,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2311,7 +2306,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2372,14 +2367,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -2418,7 +2413,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2450,7 +2445,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2476,7 +2471,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2498,7 +2493,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2524,7 +2519,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2550,7 +2545,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2576,7 +2571,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2637,14 +2632,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -2683,7 +2678,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2715,7 +2710,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2741,7 +2736,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -2767,7 +2762,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2793,7 +2788,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2819,7 +2814,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2841,7 +2836,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2902,14 +2897,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -2948,16 +2943,16 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2980,16 +2975,16 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -3012,16 +3007,16 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -3044,7 +3039,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3070,7 +3065,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -3092,7 +3087,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3118,7 +3113,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3179,14 +3174,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -3225,16 +3220,16 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3257,16 +3252,16 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -3289,15 +3284,15 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -3320,7 +3315,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3346,7 +3341,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -3368,7 +3363,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3394,7 +3389,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3455,14 +3450,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -3501,7 +3496,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3533,7 +3528,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -3559,7 +3554,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3585,7 +3580,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -3607,7 +3602,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3633,7 +3628,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3659,7 +3654,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3720,14 +3715,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -3766,7 +3761,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3798,7 +3793,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -3820,7 +3815,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3846,7 +3841,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3872,7 +3867,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3898,7 +3893,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3924,7 +3919,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>

</xml_diff>

<commit_message>
Remove deputy death notification fields (#555)
As per IN-1092.
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Death.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C330B1-457E-CC44-B08F-956DE88487A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="34400" windowHeight="21940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-35600" yWindow="1360" windowWidth="34400" windowHeight="19900" tabRatio="500" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="13" r:id="rId1"/>
@@ -20,11 +26,8 @@
     <sheet name="deputy_death_notifications" sheetId="8" r:id="rId11"/>
     <sheet name="deputy_date_of_death_lookup" sheetId="9" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -34,6 +37,9 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -42,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="91">
   <si>
     <t>casrec_code</t>
   </si>
@@ -188,18 +194,12 @@
     <t>Migrated</t>
   </si>
   <si>
-    <t>Deputy</t>
-  </si>
-  <si>
     <t>OTHER</t>
   </si>
   <si>
     <t>Migration</t>
   </si>
   <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
     <t>DECEASED</t>
   </si>
   <si>
@@ -318,16 +318,19 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -443,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -478,6 +481,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,21 +828,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="20.5" customWidth="1"/>
@@ -841,74 +851,74 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="14">
+      <c r="A2" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>77</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>79</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="H2" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14">
+      <c r="A3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="16" t="s">
-        <v>83</v>
-      </c>
       <c r="B3" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -922,7 +932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -930,7 +940,7 @@
       <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -1005,7 +1015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14">
+    <row r="2" spans="1:17" ht="15">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1026,7 +1036,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14">
+    <row r="3" spans="1:17" ht="15">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1050,7 +1060,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14">
+    <row r="4" spans="1:17" ht="16">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1075,7 +1085,7 @@
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
@@ -1084,7 +1094,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="14">
+    <row r="5" spans="1:17" ht="15">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1116,7 +1126,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="14">
+    <row r="6" spans="1:17" ht="15">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1144,7 +1154,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="14">
+    <row r="7" spans="1:17" ht="15">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -1176,7 +1186,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="14">
+    <row r="8" spans="1:17" ht="16">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1201,7 +1211,7 @@
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -1210,7 +1220,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14">
+    <row r="9" spans="1:17" ht="15">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1238,7 +1248,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14">
+    <row r="10" spans="1:17" ht="16">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1263,7 +1273,7 @@
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -1272,7 +1282,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="14">
+    <row r="11" spans="1:17" ht="15">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1315,16 +1325,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -1338,7 +1348,7 @@
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="22.5" customWidth="1"/>
     <col min="12" max="12" width="20.5" customWidth="1"/>
-    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="13" max="13" width="17.5" style="21" customWidth="1"/>
     <col min="14" max="14" width="20.5" customWidth="1"/>
     <col min="15" max="15" width="18.33203125" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" customWidth="1"/>
@@ -1383,7 +1393,7 @@
       <c r="L1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="20" t="s">
         <v>22</v>
       </c>
       <c r="N1" s="9" t="s">
@@ -1399,7 +1409,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14">
+    <row r="2" spans="1:17" ht="15">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1420,7 +1430,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14">
+    <row r="3" spans="1:17" ht="15">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1444,7 +1454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14">
+    <row r="4" spans="1:17" ht="15">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1465,17 +1475,16 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="12"/>
-      <c r="M4" s="5" t="b">
-        <f>TRUE()</f>
+      <c r="M4" s="22" t="b">
         <v>1</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1492,19 +1501,15 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="H5" s="5"/>
+      <c r="J5" s="6"/>
       <c r="K5" s="5"/>
       <c r="L5" s="13"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15">
@@ -1524,19 +1529,15 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="H6" s="5"/>
+      <c r="J6" s="6"/>
       <c r="K6" s="5"/>
       <c r="L6" s="14"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15">
@@ -1556,19 +1557,15 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="H7" s="5"/>
+      <c r="J7" s="6"/>
       <c r="K7" s="5"/>
       <c r="L7" s="14"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15">
@@ -1593,15 +1590,15 @@
       <c r="K8" s="5"/>
       <c r="L8" s="14"/>
       <c r="M8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1623,12 +1620,12 @@
       <c r="K9" s="5"/>
       <c r="L9" s="12"/>
       <c r="M9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="4" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15">
@@ -1652,16 +1649,14 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="14"/>
-      <c r="M10" s="5" t="s">
-        <v>51</v>
-      </c>
+      <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="14">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1688,7 +1683,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
     </row>
     <row r="1048576" ht="15.75" customHeight="1"/>
@@ -1704,14 +1699,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -1750,16 +1745,16 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="2">
         <v>99</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1782,7 +1777,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -1807,7 +1802,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1833,7 +1828,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1859,7 +1854,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1885,7 +1880,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1911,7 +1906,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1972,14 +1967,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X1048569"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -2027,7 +2022,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="2"/>
@@ -2050,7 +2045,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4">
         <v>3</v>
       </c>
@@ -2059,10 +2054,10 @@
         <v>5</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="14">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -2071,7 +2066,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="14">
@@ -2083,7 +2078,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="1048569" ht="15.75" customHeight="1"/>
@@ -2099,14 +2094,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
@@ -2147,13 +2142,13 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D2" s="5" t="b">
         <v>1</v>
@@ -2179,13 +2174,13 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="6" t="b">
         <v>0</v>
@@ -2211,7 +2206,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2233,7 +2228,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2259,7 +2254,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2285,7 +2280,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2311,7 +2306,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2372,14 +2367,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -2418,7 +2413,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2450,7 +2445,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2476,7 +2471,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2498,7 +2493,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2524,7 +2519,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2550,7 +2545,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -2576,7 +2571,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2637,14 +2632,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -2683,7 +2678,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2715,7 +2710,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -2741,7 +2736,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -2767,7 +2762,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -2793,7 +2788,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2819,7 +2814,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="E7" s="7"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2841,7 +2836,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2902,14 +2897,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -2948,16 +2943,16 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2980,16 +2975,16 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -3012,16 +3007,16 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -3044,7 +3039,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3070,7 +3065,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -3092,7 +3087,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3118,7 +3113,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3179,14 +3174,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -3225,16 +3220,16 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3257,16 +3252,16 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
@@ -3289,15 +3284,15 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="2"/>
@@ -3320,7 +3315,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3346,7 +3341,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -3368,7 +3363,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3394,7 +3389,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3455,14 +3450,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -3501,7 +3496,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3533,7 +3528,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -3559,7 +3554,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3585,7 +3580,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="E5" s="7"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -3607,7 +3602,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3633,7 +3628,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3659,7 +3654,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -3720,14 +3715,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -3766,7 +3761,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="14">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -3798,7 +3793,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="14">
+    <row r="3" spans="1:24" ht="15">
       <c r="E3" s="7"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -3820,7 +3815,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="14">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -3846,7 +3841,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="14">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3872,7 +3867,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="14">
+    <row r="6" spans="1:24" ht="15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3898,7 +3893,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="14">
+    <row r="7" spans="1:24" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -3924,7 +3919,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="13">
+    <row r="8" spans="1:24" ht="14">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>

</xml_diff>